<commit_message>
Update CROSS SECTIONAL STUDY DATA_v2.xlsx
</commit_message>
<xml_diff>
--- a/Data Preprocessing/CROSS SECTIONAL STUDY DATA_v2.xlsx
+++ b/Data Preprocessing/CROSS SECTIONAL STUDY DATA_v2.xlsx
@@ -800,9 +800,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="Z18" sqref="Z18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>